<commit_message>
antes de mover sesiones
</commit_message>
<xml_diff>
--- a/web/reportes/comparativo-9-11.xlsx
+++ b/web/reportes/comparativo-9-11.xlsx
@@ -637,9 +637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8:H997"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>